<commit_message>
Atualiza carro, recomeca, atualiza texto
</commit_message>
<xml_diff>
--- a/documentacao/backlog.xlsx
+++ b/documentacao/backlog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t>lista de tarefas</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>f1_main.js</t>
+  </si>
+  <si>
+    <t>f1_class.js</t>
   </si>
 </sst>
 </file>
@@ -948,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1165,7 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
         <v>40</v>

</xml_diff>